<commit_message>
Update column names from physical quantity to measurand
</commit_message>
<xml_diff>
--- a/data/misused_bar_graph_figures/acs_nano/log/annotation.xlsx
+++ b/data/misused_bar_graph_figures/acs_nano/log/annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlin/Files/2023-2028-UC_Berkeley/_landry-lab/research-project/local/misused-bar-graphs/data/misused_bar_graph_figures/acs_nano/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB583CBF-4F37-AD41-A353-2BFB6E534FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF4DC0D-95B8-374F-9C1E-60EB46EC3587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="740" windowWidth="14300" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="500" windowWidth="37600" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -235,9 +235,6 @@
     <t>10.1021:acsnano.3c10225</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Concentration by PM (ng/mL)</t>
   </si>
   <si>
@@ -451,12 +448,6 @@
     <t>Concentration</t>
   </si>
   <si>
-    <t>Physical quantity I</t>
-  </si>
-  <si>
-    <t>Physical quantity II</t>
-  </si>
-  <si>
     <t>Measured value</t>
   </si>
   <si>
@@ -881,6 +872,15 @@
   </si>
   <si>
     <t>10.1021:acsnano.3c00958_log_fig1</t>
+  </si>
+  <si>
+    <t>Measurand</t>
+  </si>
+  <si>
+    <t>Measurand Level I</t>
+  </si>
+  <si>
+    <t>Measurand Level II</t>
   </si>
 </sst>
 </file>
@@ -1284,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="187" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1302,7 +1302,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1317,30 +1317,30 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>71</v>
+        <v>284</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1352,27 +1352,27 @@
         <v>7</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1387,27 +1387,27 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1422,27 +1422,27 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -1457,27 +1457,27 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1492,27 +1492,27 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -1527,27 +1527,27 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -1562,27 +1562,27 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -1597,27 +1597,27 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I9" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J9" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -1632,27 +1632,27 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -1667,27 +1667,27 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -1702,27 +1702,27 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -1737,27 +1737,27 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1772,27 +1772,27 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -1807,27 +1807,27 @@
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -1842,27 +1842,27 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -1877,27 +1877,27 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1912,27 +1912,27 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -1947,27 +1947,27 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -1982,27 +1982,27 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H20" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -2017,27 +2017,27 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K21" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -2052,27 +2052,27 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
@@ -2087,27 +2087,27 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I23" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J23" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -2122,27 +2122,27 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I24" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -2157,27 +2157,27 @@
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -2192,27 +2192,27 @@
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I26" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J26" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -2227,27 +2227,27 @@
         <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I27" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -2262,27 +2262,27 @@
         <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -2297,27 +2297,27 @@
         <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I29" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J29" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -2332,27 +2332,27 @@
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J30" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K30" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -2367,27 +2367,27 @@
         <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -2402,27 +2402,27 @@
         <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G32" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K32" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
@@ -2437,27 +2437,27 @@
         <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K33" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
@@ -2472,27 +2472,27 @@
         <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H34" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I34" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J34" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K34" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
@@ -2507,27 +2507,27 @@
         <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H35" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K35" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B36" t="s">
         <v>33</v>
@@ -2542,27 +2542,27 @@
         <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H36" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I36" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K36" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B37" t="s">
         <v>33</v>
@@ -2577,30 +2577,30 @@
         <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G37" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H37" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I37" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J37" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K37" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B38" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -2612,27 +2612,27 @@
         <v>7</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G38" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K38" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B39" t="s">
         <v>34</v>
@@ -2647,27 +2647,27 @@
         <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H39" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I39" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B40" t="s">
         <v>34</v>
@@ -2682,27 +2682,27 @@
         <v>7</v>
       </c>
       <c r="F40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H40" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I40" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K40" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B41" t="s">
         <v>34</v>
@@ -2717,27 +2717,27 @@
         <v>7</v>
       </c>
       <c r="F41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I41" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B42" t="s">
         <v>34</v>
@@ -2752,27 +2752,27 @@
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I42" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K42" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -2787,27 +2787,27 @@
         <v>7</v>
       </c>
       <c r="F43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G43" t="s">
+        <v>144</v>
+      </c>
+      <c r="H43" t="s">
+        <v>154</v>
+      </c>
+      <c r="I43" t="s">
+        <v>159</v>
+      </c>
+      <c r="J43" t="s">
         <v>147</v>
       </c>
-      <c r="H43" t="s">
-        <v>157</v>
-      </c>
-      <c r="I43" t="s">
-        <v>162</v>
-      </c>
-      <c r="J43" t="s">
-        <v>150</v>
-      </c>
       <c r="K43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B44" t="s">
         <v>36</v>
@@ -2822,27 +2822,27 @@
         <v>7</v>
       </c>
       <c r="F44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I44" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J44" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B45" t="s">
         <v>36</v>
@@ -2857,27 +2857,27 @@
         <v>7</v>
       </c>
       <c r="F45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I45" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J45" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K45" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B46" t="s">
         <v>36</v>
@@ -2892,27 +2892,27 @@
         <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H46" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I46" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J46" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K46" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B47" t="s">
         <v>36</v>
@@ -2927,27 +2927,27 @@
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H47" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I47" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J47" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K47" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B48" t="s">
         <v>37</v>
@@ -2962,27 +2962,27 @@
         <v>7</v>
       </c>
       <c r="F48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H48" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I48" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J48" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K48" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B49" t="s">
         <v>38</v>
@@ -2997,27 +2997,27 @@
         <v>7</v>
       </c>
       <c r="F49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H49" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I49" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K49" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B50" t="s">
         <v>38</v>
@@ -3032,27 +3032,27 @@
         <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G50" t="s">
+        <v>144</v>
+      </c>
+      <c r="H50" t="s">
+        <v>154</v>
+      </c>
+      <c r="I50" t="s">
+        <v>159</v>
+      </c>
+      <c r="J50" t="s">
         <v>147</v>
       </c>
-      <c r="H50" t="s">
-        <v>157</v>
-      </c>
-      <c r="I50" t="s">
-        <v>162</v>
-      </c>
-      <c r="J50" t="s">
-        <v>150</v>
-      </c>
       <c r="K50" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B51" t="s">
         <v>39</v>
@@ -3067,27 +3067,27 @@
         <v>7</v>
       </c>
       <c r="F51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H51" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I51" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K51" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B52" t="s">
         <v>39</v>
@@ -3102,27 +3102,27 @@
         <v>7</v>
       </c>
       <c r="F52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H52" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I52" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K52" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B53" t="s">
         <v>39</v>
@@ -3137,27 +3137,27 @@
         <v>7</v>
       </c>
       <c r="F53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H53" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I53" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K53" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B54" t="s">
         <v>39</v>
@@ -3172,27 +3172,27 @@
         <v>7</v>
       </c>
       <c r="F54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H54" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I54" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K54" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B55" t="s">
         <v>39</v>
@@ -3207,27 +3207,27 @@
         <v>7</v>
       </c>
       <c r="F55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H55" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I55" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B56" t="s">
         <v>39</v>
@@ -3242,27 +3242,27 @@
         <v>7</v>
       </c>
       <c r="F56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H56" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I56" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K56" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B57" t="s">
         <v>39</v>
@@ -3277,27 +3277,27 @@
         <v>7</v>
       </c>
       <c r="F57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H57" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I57" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B58" t="s">
         <v>39</v>
@@ -3312,27 +3312,27 @@
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H58" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I58" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K58" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B59" t="s">
         <v>39</v>
@@ -3347,27 +3347,27 @@
         <v>7</v>
       </c>
       <c r="F59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H59" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I59" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K59" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B60" t="s">
         <v>39</v>
@@ -3382,27 +3382,27 @@
         <v>7</v>
       </c>
       <c r="F60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H60" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I60" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K60" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B61" t="s">
         <v>39</v>
@@ -3417,27 +3417,27 @@
         <v>7</v>
       </c>
       <c r="F61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H61" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I61" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K61" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B62" t="s">
         <v>46</v>
@@ -3452,27 +3452,27 @@
         <v>7</v>
       </c>
       <c r="F62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G62" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H62" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I62" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J62" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K62" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B63" t="s">
         <v>47</v>
@@ -3487,27 +3487,27 @@
         <v>7</v>
       </c>
       <c r="F63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H63" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I63" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K63" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B64" t="s">
         <v>48</v>
@@ -3522,27 +3522,27 @@
         <v>7</v>
       </c>
       <c r="F64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G64" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H64" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J64" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K64" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B65" t="s">
         <v>48</v>
@@ -3557,27 +3557,27 @@
         <v>7</v>
       </c>
       <c r="F65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H65" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J65" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K65" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B66" t="s">
         <v>48</v>
@@ -3592,27 +3592,27 @@
         <v>7</v>
       </c>
       <c r="F66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H66" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J66" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K66" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B67" t="s">
         <v>49</v>
@@ -3627,27 +3627,27 @@
         <v>7</v>
       </c>
       <c r="F67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G67" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H67" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I67" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J67" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B68" t="s">
         <v>49</v>
@@ -3662,27 +3662,27 @@
         <v>7</v>
       </c>
       <c r="F68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H68" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I68" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J68" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K68" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B69" t="s">
         <v>50</v>
@@ -3697,27 +3697,27 @@
         <v>7</v>
       </c>
       <c r="F69" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H69" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I69" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K69" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B70" t="s">
         <v>50</v>
@@ -3732,27 +3732,27 @@
         <v>7</v>
       </c>
       <c r="F70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H70" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I70" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K70" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B71" t="s">
         <v>51</v>
@@ -3767,27 +3767,27 @@
         <v>7</v>
       </c>
       <c r="F71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I71" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J71" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K71" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
@@ -3802,27 +3802,27 @@
         <v>7</v>
       </c>
       <c r="F72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H72" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I72" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J72" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K72" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
@@ -3837,27 +3837,27 @@
         <v>7</v>
       </c>
       <c r="F73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H73" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I73" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J73" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K73" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B74" t="s">
         <v>53</v>
@@ -3872,27 +3872,27 @@
         <v>7</v>
       </c>
       <c r="F74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G74" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H74" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I74" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J74" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K74" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B75" t="s">
         <v>54</v>
@@ -3907,27 +3907,27 @@
         <v>7</v>
       </c>
       <c r="F75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H75" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I75" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J75" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K75" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B76" t="s">
         <v>54</v>
@@ -3942,27 +3942,27 @@
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H76" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I76" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J76" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K76" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B77" t="s">
         <v>55</v>
@@ -3977,27 +3977,27 @@
         <v>7</v>
       </c>
       <c r="F77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H77" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I77" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J77" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K77" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B78" t="s">
         <v>55</v>
@@ -4012,27 +4012,27 @@
         <v>7</v>
       </c>
       <c r="F78" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H78" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I78" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J78" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K78" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B79" t="s">
         <v>55</v>
@@ -4047,27 +4047,27 @@
         <v>7</v>
       </c>
       <c r="F79" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G79" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H79" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I79" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J79" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K79" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B80" t="s">
         <v>55</v>
@@ -4082,27 +4082,27 @@
         <v>7</v>
       </c>
       <c r="F80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G80" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H80" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I80" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J80" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K80" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B81" t="s">
         <v>55</v>
@@ -4117,27 +4117,27 @@
         <v>7</v>
       </c>
       <c r="F81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H81" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I81" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J81" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K81" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B82" t="s">
         <v>55</v>
@@ -4152,27 +4152,27 @@
         <v>7</v>
       </c>
       <c r="F82" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G82" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H82" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I82" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J82" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K82" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B83" t="s">
         <v>56</v>
@@ -4187,27 +4187,27 @@
         <v>7</v>
       </c>
       <c r="F83" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H83" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I83" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J83" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K83" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B84" t="s">
         <v>57</v>
@@ -4222,27 +4222,27 @@
         <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G84" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H84" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I84" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J84" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K84" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B85" t="s">
         <v>58</v>
@@ -4257,27 +4257,27 @@
         <v>7</v>
       </c>
       <c r="F85" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G85" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H85" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I85" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J85" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K85" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B86" t="s">
         <v>58</v>
@@ -4292,27 +4292,27 @@
         <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G86" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H86" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I86" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J86" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K86" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B87" t="s">
         <v>58</v>
@@ -4327,27 +4327,27 @@
         <v>7</v>
       </c>
       <c r="F87" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G87" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H87" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I87" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J87" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K87" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B88" t="s">
         <v>58</v>
@@ -4362,27 +4362,27 @@
         <v>7</v>
       </c>
       <c r="F88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G88" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H88" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I88" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J88" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K88" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B89" t="s">
         <v>58</v>
@@ -4397,27 +4397,27 @@
         <v>7</v>
       </c>
       <c r="F89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G89" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H89" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I89" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J89" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K89" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B90" t="s">
         <v>58</v>
@@ -4432,27 +4432,27 @@
         <v>7</v>
       </c>
       <c r="F90" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G90" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H90" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I90" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J90" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K90" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B91" t="s">
         <v>58</v>
@@ -4467,27 +4467,27 @@
         <v>7</v>
       </c>
       <c r="F91" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G91" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H91" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I91" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J91" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K91" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B92" t="s">
         <v>58</v>
@@ -4502,27 +4502,27 @@
         <v>7</v>
       </c>
       <c r="F92" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H92" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I92" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J92" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K92" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B93" t="s">
         <v>58</v>
@@ -4537,27 +4537,27 @@
         <v>7</v>
       </c>
       <c r="F93" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G93" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H93" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I93" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J93" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K93" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B94" t="s">
         <v>58</v>
@@ -4572,27 +4572,27 @@
         <v>7</v>
       </c>
       <c r="F94" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G94" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H94" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I94" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J94" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K94" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B95" t="s">
         <v>59</v>
@@ -4607,27 +4607,27 @@
         <v>7</v>
       </c>
       <c r="F95" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G95" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H95" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I95" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J95" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K95" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B96" t="s">
         <v>60</v>
@@ -4642,27 +4642,27 @@
         <v>7</v>
       </c>
       <c r="F96" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G96" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H96" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I96" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J96" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K96" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B97" t="s">
         <v>61</v>
@@ -4677,27 +4677,27 @@
         <v>7</v>
       </c>
       <c r="F97" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G97" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H97" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I97" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J97" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K97" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B98" t="s">
         <v>61</v>
@@ -4712,27 +4712,27 @@
         <v>7</v>
       </c>
       <c r="F98" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G98" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H98" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I98" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J98" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K98" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B99" t="s">
         <v>61</v>
@@ -4747,27 +4747,27 @@
         <v>7</v>
       </c>
       <c r="F99" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G99" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H99" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I99" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J99" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K99" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B100" t="s">
         <v>62</v>
@@ -4782,27 +4782,27 @@
         <v>7</v>
       </c>
       <c r="F100" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G100" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H100" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I100" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J100" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K100" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B101" t="s">
         <v>62</v>
@@ -4817,27 +4817,27 @@
         <v>7</v>
       </c>
       <c r="F101" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G101" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H101" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I101" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J101" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K101" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B102" t="s">
         <v>63</v>
@@ -4852,27 +4852,27 @@
         <v>7</v>
       </c>
       <c r="F102" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G102" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H102" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I102" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J102" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K102" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B103" t="s">
         <v>64</v>
@@ -4887,27 +4887,27 @@
         <v>7</v>
       </c>
       <c r="F103" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G103" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H103" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I103" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J103" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K103" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
         <v>64</v>
@@ -4922,27 +4922,27 @@
         <v>7</v>
       </c>
       <c r="F104" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G104" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H104" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I104" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J104" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K104" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B105" t="s">
         <v>65</v>
@@ -4957,27 +4957,27 @@
         <v>7</v>
       </c>
       <c r="F105" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G105" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H105" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I105" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J105" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K105" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B106" t="s">
         <v>66</v>
@@ -4992,27 +4992,27 @@
         <v>7</v>
       </c>
       <c r="F106" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G106" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H106" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I106" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J106" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K106" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B107" t="s">
         <v>66</v>
@@ -5027,27 +5027,27 @@
         <v>7</v>
       </c>
       <c r="F107" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G107" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H107" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I107" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J107" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K107" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B108" t="s">
         <v>66</v>
@@ -5062,27 +5062,27 @@
         <v>7</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H108" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I108" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J108" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K108" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B109" t="s">
         <v>66</v>
@@ -5097,27 +5097,27 @@
         <v>7</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G109" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H109" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I109" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J109" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K109" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B110" t="s">
         <v>67</v>
@@ -5132,27 +5132,27 @@
         <v>7</v>
       </c>
       <c r="F110" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G110" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H110" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I110" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J110" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K110" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B111" t="s">
         <v>68</v>
@@ -5167,27 +5167,27 @@
         <v>7</v>
       </c>
       <c r="F111" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G111" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H111" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I111" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J111" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K111" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B112" t="s">
         <v>69</v>
@@ -5202,27 +5202,27 @@
         <v>7</v>
       </c>
       <c r="F112" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G112" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H112" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I112" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J112" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K112" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B113" t="s">
         <v>70</v>
@@ -5237,22 +5237,22 @@
         <v>7</v>
       </c>
       <c r="F113" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G113" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H113" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I113" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J113" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K113" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>